<commit_message>
refdata & sort for baseschema
[generate-fake-db]
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/refdata-valid.xlsx
+++ b/packages/central-server/__tests__/importers/refdata-valid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flynnteh/BES/tamanu/packages/central-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB170F5-B12B-DF47-853B-EFD5B55F9D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAF8675-F80F-2E4C-846F-0CCBDEC58277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25460" windowHeight="17500" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="569">
   <si>
     <t>id</t>
   </si>
@@ -1832,6 +1832,9 @@
   </si>
   <si>
     <t>doseLabel</t>
+  </si>
+  <si>
+    <t>sort</t>
   </si>
 </sst>
 </file>
@@ -16528,10 +16531,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16542,13 +16545,13 @@
     <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.6640625" style="1"/>
+    <col min="7" max="8" width="10.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -16570,11 +16573,14 @@
       <c r="G1" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="13" t="s">
+        <v>568</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>555</v>
       </c>
@@ -16592,11 +16598,14 @@
       <c r="G2" s="9">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="9">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -16605,8 +16614,9 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -16615,8 +16625,9 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -16625,8 +16636,9 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -16635,8 +16647,9 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -16645,8 +16658,9 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -16655,8 +16669,9 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -16665,8 +16680,9 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -16675,6 +16691,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51181100000000002" footer="0.51181100000000002"/>

</xml_diff>

<commit_message>
nass-1155: how many merge gone wrong :cry
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/refdata-valid.xlsx
+++ b/packages/central-server/__tests__/importers/refdata-valid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flynnteh/BES/tamanu/packages/central-server/__tests__/importers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAF8675-F80F-2E4C-846F-0CCBDEC58277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B7036B-7E96-E042-8E2A-FFB06FFD0722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25460" windowHeight="17500" firstSheet="10" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1834,7 +1834,7 @@
     <t>doseLabel</t>
   </si>
   <si>
-    <t>sort</t>
+    <t>sortIndex</t>
   </si>
 </sst>
 </file>
@@ -16533,8 +16533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>